<commit_message>
Update to China inventory scaling 1. Add mapping file for NOx. Don't scale CEDS AGR NOx emissions to regional inventory (value of zero). This corrects for a previous underprediction in AGR NOx.
</commit_message>
<xml_diff>
--- a/input/mappings/scaling/MEIC_2017Update_scaling_mapping.xlsx
+++ b/input/mappings/scaling/MEIC_2017Update_scaling_mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11013"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emcduffie/Documents/GEOS-Chem/CEDS_Emissions/CEDS_v0611/input/mappings/scaling/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emcduffie/Documents/GEOS-Chem/CEDS/CEDS_v0611/input/mappings/scaling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE397A86-0319-C041-BF4C-AC24E927051C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D235E2EF-F503-C348-9AF9-D4B8707ADFE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24320" yWindow="2060" windowWidth="14040" windowHeight="14600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9000" yWindow="2260" windowWidth="18420" windowHeight="15400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="map" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="117">
   <si>
     <t>1A1a_Electricity-public</t>
   </si>
@@ -180,72 +180,18 @@
     <t>power</t>
   </si>
   <si>
-    <t>heating</t>
-  </si>
-  <si>
     <t>industrial boiler</t>
   </si>
   <si>
-    <t>onroad</t>
-  </si>
-  <si>
-    <t>rail</t>
-  </si>
-  <si>
-    <t>inland waterway</t>
-  </si>
-  <si>
-    <t>other offroad</t>
-  </si>
-  <si>
     <t>residential</t>
   </si>
   <si>
     <t>cement</t>
   </si>
   <si>
-    <t>lime</t>
-  </si>
-  <si>
-    <t>brick and glass</t>
-  </si>
-  <si>
-    <t>inorganic / organic chemicals production</t>
-  </si>
-  <si>
     <t>iron and steel</t>
   </si>
   <si>
-    <t>aluminum</t>
-  </si>
-  <si>
-    <t>other non-ferrous</t>
-  </si>
-  <si>
-    <t>domestic solvent use, dry clean, priting gasoline cleaning</t>
-  </si>
-  <si>
-    <t>paint application</t>
-  </si>
-  <si>
-    <t>printing ink, passenger vehicle treated, pesticle use, glue use</t>
-  </si>
-  <si>
-    <t>pulp, food, beverage, wood</t>
-  </si>
-  <si>
-    <t>manure management</t>
-  </si>
-  <si>
-    <t>fertilizer</t>
-  </si>
-  <si>
-    <t>waste disposal</t>
-  </si>
-  <si>
-    <t>waste incineration</t>
-  </si>
-  <si>
     <t>iso</t>
   </si>
   <si>
@@ -418,6 +364,27 @@
   </si>
   <si>
     <t>IPCC codes</t>
+  </si>
+  <si>
+    <t>heating (residential &amp; industrial)</t>
+  </si>
+  <si>
+    <t>industrial boiler/iron&amp;steel</t>
+  </si>
+  <si>
+    <t>industrial broiler</t>
+  </si>
+  <si>
+    <t>onroad/motorcyle</t>
+  </si>
+  <si>
+    <t>other industry</t>
+  </si>
+  <si>
+    <t>other industry/iron &amp; steel</t>
+  </si>
+  <si>
+    <t>solvents (residential &amp; industrial)</t>
   </si>
 </sst>
 </file>
@@ -481,7 +448,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -491,12 +458,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -640,7 +601,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -649,13 +610,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1063,11 +1023,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E66"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B59" sqref="B59"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1080,22 +1040,22 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="D1" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="E1"/>
     </row>
     <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
         <v>47</v>
@@ -1103,50 +1063,53 @@
       <c r="C2" t="s">
         <v>0</v>
       </c>
+      <c r="D2" t="s">
+        <v>47</v>
+      </c>
       <c r="E2"/>
     </row>
     <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="E3"/>
     </row>
     <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E4"/>
     </row>
     <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="E5"/>
     </row>
     <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="B6" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="E6"/>
     </row>
     <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="B7" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="E7"/>
     </row>
@@ -1163,155 +1126,194 @@
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>47</v>
       </c>
       <c r="C9" t="s">
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>92</v>
+      <c r="B10" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="C10" t="s">
         <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>110</v>
       </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="4" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>111</v>
       </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="4" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>112</v>
       </c>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="4" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>112</v>
       </c>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>112</v>
       </c>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="4" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>7</v>
+      </c>
+      <c r="D15" t="s">
+        <v>112</v>
       </c>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="4" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="D16" t="s">
+        <v>112</v>
+      </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B17" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C17" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>112</v>
       </c>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="4" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>10</v>
+      </c>
+      <c r="D18" t="s">
+        <v>112</v>
       </c>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="4" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>11</v>
+      </c>
+      <c r="D19" t="s">
+        <v>112</v>
       </c>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="4" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>12</v>
+      </c>
+      <c r="D20" t="s">
+        <v>112</v>
       </c>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="4" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>13</v>
+      </c>
+      <c r="D21" t="s">
+        <v>112</v>
       </c>
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="4" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="D22" t="s">
+        <v>112</v>
+      </c>
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="6"/>
+      <c r="A23" s="5"/>
       <c r="B23" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C23" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>15</v>
+      </c>
+      <c r="D23" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1328,377 +1330,356 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="C26" t="s">
         <v>41</v>
       </c>
       <c r="D26" t="s">
-        <v>50</v>
+        <v>113</v>
       </c>
       <c r="E26" s="1"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="C27" t="s">
         <v>16</v>
       </c>
       <c r="D27" t="s">
-        <v>51</v>
+        <v>100</v>
       </c>
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
-        <v>93</v>
-      </c>
       <c r="C28" t="s">
         <v>17</v>
       </c>
       <c r="E28" s="1"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
-        <v>93</v>
-      </c>
       <c r="C29" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="C30" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="D30" t="s">
-        <v>52</v>
+        <v>100</v>
       </c>
       <c r="E30" s="1"/>
     </row>
-    <row r="31" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31"/>
       <c r="B31" t="s">
-        <v>93</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E31" s="9"/>
-    </row>
-    <row r="32" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" t="s">
+        <v>100</v>
+      </c>
+      <c r="E31" s="8"/>
+    </row>
+    <row r="32" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32"/>
       <c r="B32" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C32" t="s">
         <v>42</v>
       </c>
-      <c r="D32"/>
-      <c r="E32" s="9"/>
+      <c r="D32" t="s">
+        <v>91</v>
+      </c>
+      <c r="E32" s="8"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C33" t="s">
         <v>43</v>
       </c>
       <c r="D33" t="s">
-        <v>54</v>
+        <v>91</v>
       </c>
       <c r="E33" s="1"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C34" t="s">
-        <v>97</v>
+        <v>79</v>
+      </c>
+      <c r="D34" t="s">
+        <v>91</v>
       </c>
       <c r="E34" s="1"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C35" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="E35" s="1"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="C36" t="s">
         <v>44</v>
       </c>
+      <c r="D36" t="s">
+        <v>114</v>
+      </c>
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="C37" t="s">
-        <v>82</v>
+        <v>64</v>
+      </c>
+      <c r="D37" t="s">
+        <v>114</v>
       </c>
       <c r="E37" s="1"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="C38" t="s">
         <v>18</v>
       </c>
+      <c r="D38" t="s">
+        <v>114</v>
+      </c>
       <c r="E38" s="1"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="C39" t="s">
         <v>19</v>
       </c>
       <c r="D39" t="s">
-        <v>55</v>
+        <v>114</v>
       </c>
       <c r="E39" s="1"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="C40" t="s">
         <v>20</v>
       </c>
       <c r="D40" t="s">
-        <v>56</v>
+        <v>114</v>
       </c>
       <c r="E40" s="1"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="C41" t="s">
         <v>21</v>
       </c>
       <c r="D41" t="s">
-        <v>57</v>
+        <v>114</v>
       </c>
       <c r="E41" s="1"/>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="C42" t="s">
         <v>22</v>
       </c>
       <c r="D42" t="s">
-        <v>58</v>
+        <v>114</v>
       </c>
       <c r="E42" s="1"/>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="C43" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="D43" t="s">
-        <v>59</v>
+        <v>115</v>
       </c>
       <c r="E43" s="1"/>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B44" s="5"/>
+      <c r="B44" t="s">
+        <v>76</v>
+      </c>
+      <c r="C44" t="s">
+        <v>33</v>
+      </c>
       <c r="D44" t="s">
-        <v>60</v>
-      </c>
-      <c r="E44" s="1"/>
+        <v>116</v>
+      </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B45" s="5"/>
+      <c r="B45" t="s">
+        <v>76</v>
+      </c>
+      <c r="C45" t="s">
+        <v>65</v>
+      </c>
       <c r="D45" t="s">
-        <v>61</v>
-      </c>
-      <c r="E45" s="1"/>
+        <v>116</v>
+      </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="C46" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D46" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="C47" t="s">
-        <v>83</v>
+        <v>34</v>
       </c>
       <c r="D47" t="s">
-        <v>64</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="E47" s="9"/>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="C48" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D48" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B49" t="s">
-        <v>94</v>
-      </c>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C49" t="s">
-        <v>34</v>
-      </c>
-      <c r="E49" s="10"/>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="C50" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D50" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="C51" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B52" t="s">
-        <v>95</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="D51" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C52" t="s">
-        <v>38</v>
-      </c>
-      <c r="D52" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B53" t="s">
-        <v>95</v>
-      </c>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C53" t="s">
-        <v>39</v>
-      </c>
-      <c r="D53" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B54" t="s">
-        <v>95</v>
-      </c>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C54" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B55" t="s">
-        <v>95</v>
-      </c>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C55" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D55" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B56" t="s">
-        <v>95</v>
-      </c>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C56" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C57" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D57" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C58" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C59" t="s">
-        <v>26</v>
-      </c>
-      <c r="D59" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C60" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B61" t="s">
-        <v>92</v>
-      </c>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C61" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C62" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C63" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C64" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C65" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C66" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1731,36 +1712,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="D1" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="E1" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="E2" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1785,30 +1766,30 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="D1" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1833,200 +1814,200 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="C3" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="D3" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="11"/>
+      <c r="B5" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="11"/>
+      <c r="B6" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="11"/>
+      <c r="B7" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="11"/>
+      <c r="B8" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="11"/>
+      <c r="B9" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="11"/>
+      <c r="B10" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="11"/>
+      <c r="B11" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="11"/>
+      <c r="B12" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="11"/>
+      <c r="B13" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="11"/>
+      <c r="B14" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="11"/>
+      <c r="B15" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="11"/>
+      <c r="B16" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="11" t="s">
+      <c r="C16" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="11"/>
+      <c r="B17" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D17" s="12" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="12"/>
-      <c r="B5" s="13" t="s">
+    <row r="18" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
+      <c r="B18" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="C5" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="D5" s="13" t="s">
+      <c r="C18" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="14" t="s">
         <v>106</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="12"/>
-      <c r="B6" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="12"/>
-      <c r="B7" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="12"/>
-      <c r="B8" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="12"/>
-      <c r="B9" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="12"/>
-      <c r="B11" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="12"/>
-      <c r="B12" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="12"/>
-      <c r="B13" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="12"/>
-      <c r="B14" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="12"/>
-      <c r="B15" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="D15" s="13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="12"/>
-      <c r="B16" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" s="13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="12"/>
-      <c r="B17" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>